<commit_message>
Update the example call task.
</commit_message>
<xml_diff>
--- a/contract_flow/call_job.xlsx
+++ b/contract_flow/call_job.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrus/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89336346-D939-864B-BA82-588B0DA9005B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5F1C0D-8F70-5342-832C-E90F80669155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="27320" windowHeight="14900" activeTab="2" xr2:uid="{1F2E5FC9-343A-4109-8460-8F9B64DB7B0B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" activeTab="2" xr2:uid="{1F2E5FC9-343A-4109-8460-8F9B64DB7B0B}"/>
   </bookViews>
   <sheets>
     <sheet name="configures" sheetId="3" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>Yes/No</t>
   </si>
   <si>
-    <t>How do you know Amazon Connect? A. News Letter, B. Social Media, C. AWS Event, D. AWS Website, or E. Friend.</t>
-  </si>
-  <si>
     <t>Multiple Choice</t>
   </si>
   <si>
@@ -113,17 +110,27 @@
     <t>The date for us to call you back.</t>
   </si>
   <si>
-    <t>What time will you prefer for the callback?</t>
+    <t>How do you know Amazon Connect? A. News Letter, B. Social Media, C. AWS Event, D. AWS Website, or E. From Friend.</t>
+  </si>
+  <si>
+    <t>Preferred call back time?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,11 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +503,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -519,10 +527,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -535,7 +543,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -562,34 +570,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -610,7 +618,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
rename config to configuration.
</commit_message>
<xml_diff>
--- a/contract_flow/call_job.xlsx
+++ b/contract_flow/call_job.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrus/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyrus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5F1C0D-8F70-5342-832C-E90F80669155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2592B5E9-C309-461C-9936-FB06CF8EAC4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" activeTab="2" xr2:uid="{1F2E5FC9-343A-4109-8460-8F9B64DB7B0B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{1F2E5FC9-343A-4109-8460-8F9B64DB7B0B}"/>
   </bookViews>
   <sheets>
-    <sheet name="configures" sheetId="3" r:id="rId1"/>
+    <sheet name="configuration" sheetId="3" r:id="rId1"/>
     <sheet name="questions" sheetId="1" r:id="rId2"/>
     <sheet name="receivers" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>question_template</t>
   </si>
@@ -56,9 +56,6 @@
     <t>ending</t>
   </si>
   <si>
-    <t>Hi {{ username }}, This is a simple survey.</t>
-  </si>
-  <si>
     <t>Good Bye {{ username }} and have a nice day!</t>
   </si>
   <si>
@@ -114,6 +111,12 @@
   </si>
   <si>
     <t>Preferred call back time?</t>
+  </si>
+  <si>
+    <t>This is a reminder to let you know that the book report assignment is due this Friday, 3 June 2020.  Are you ready?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi {{ username }}, </t>
   </si>
 </sst>
 </file>
@@ -168,12 +171,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,47 +501,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7151CD6-5862-49CD-A293-C653E9E9F12B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -540,72 +551,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAA08A9-03A3-4210-AD4D-D2C886E07ECD}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -617,17 +636,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCC801B-5D58-43C7-8BE7-E4D984E56CD7}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -638,7 +657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -646,10 +665,10 @@
         <v>12345678</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -657,7 +676,7 @@
         <v>89654201</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>